<commit_message>
g11.1 - correção na filtragem de linhas da tabela do siconfi
</commit_message>
<xml_diff>
--- a/Data/g11.1.xlsx
+++ b/Data/g11.1.xlsx
@@ -502,7 +502,7 @@
         <v>-0.9998837299406205</v>
       </c>
       <c r="C6" t="n">
-        <v>3.649254904281829</v>
+        <v>2.304852536422208</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>4.30376910786725</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7504482553129188</v>
+        <v>1.405387579332751</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>1.251393607016049</v>
       </c>
       <c r="C8" t="n">
-        <v>10.37676725860104</v>
+        <v>10.81400072294023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correção no script e atualização das bases
</commit_message>
<xml_diff>
--- a/Data/g11.1.xlsx
+++ b/Data/g11.1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,6 +527,17 @@
         <v>10.81400072294023</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3.118144130554446</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6.515074339641291</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>